<commit_message>
adds IFS to demo 3
</commit_message>
<xml_diff>
--- a/excel03.xlsx
+++ b/excel03.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/galvanize/TTP/EXCEL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF40D942-CA3F-4D41-A492-BF110370ECB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B0D2B22D-F047-46CA-9406-C0B2AC74B0EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="1340" windowWidth="27000" windowHeight="13380" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="1340" windowWidth="27000" windowHeight="13380" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Topics" sheetId="3" r:id="rId1"/>
     <sheet name="MAXIFS MINIFS" sheetId="1" r:id="rId2"/>
     <sheet name="MAXIFS MINIFS (an)" sheetId="4" r:id="rId3"/>
     <sheet name="IFS" sheetId="2" r:id="rId4"/>
-    <sheet name="IFS (an)" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
@@ -36,8 +35,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2504" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2494" uniqueCount="64">
   <si>
     <t>Highline Excel 2016 Class 07 Excel 2016 MAXIFS, MINIFS &amp; IFS Functions for Conditional Calculations</t>
   </si>
@@ -195,30 +216,7 @@
     <t>without nesting multiple IF functions</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">No </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>value_if_false</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>!!!!! (Must use "Last Argument TRUE Trick")</t>
-    </r>
+    <t>(Must use "Last Argument TRUE Trick")</t>
   </si>
   <si>
     <t>IFS is good when you have multiple tests and multiple results</t>
@@ -227,25 +225,19 @@
     <t>IFS is good when you have three or more items to put in a cell</t>
   </si>
   <si>
-    <t xml:space="preserve">Income Statement </t>
+    <t>Report Card</t>
   </si>
   <si>
-    <t>for Month Ended Dec 31, 2016</t>
+    <t>Score</t>
   </si>
   <si>
-    <t>Revenue</t>
-  </si>
-  <si>
-    <t>Expenses</t>
-  </si>
-  <si>
-    <t>Profit</t>
+    <t>Letter Grade</t>
   </si>
   <si>
     <t>Before IFS, We had to Nest Multiple IF functions</t>
   </si>
   <si>
-    <t>With IFS</t>
+    <t>With IFS, Can just nest them within one statement</t>
   </si>
   <si>
     <t>For more about IFS, watch this video:</t>
@@ -258,9 +250,6 @@
   </si>
   <si>
     <t>How to get Excel 2016 "Insider Program":</t>
-  </si>
-  <si>
-    <t>IFS is good when you three or more items to put in a cell</t>
   </si>
 </sst>
 </file>
@@ -369,7 +358,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -483,54 +472,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -539,7 +480,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1">
       <alignment wrapText="1"/>
@@ -557,10 +498,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="42" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -573,12 +510,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="DarkBlue" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -922,7 +855,7 @@
       <c r="B1" s="8"/>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="14" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="8"/>
@@ -931,7 +864,7 @@
       <c r="A4" s="4">
         <v>1</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="15" t="s">
         <v>2</v>
       </c>
     </row>
@@ -939,7 +872,7 @@
       <c r="A5" s="4">
         <v>2</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="15" t="s">
         <v>3</v>
       </c>
     </row>
@@ -947,7 +880,7 @@
       <c r="A6" s="4">
         <v>3</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="15" t="s">
         <v>4</v>
       </c>
     </row>
@@ -961,7 +894,7 @@
   <sheetPr>
     <tabColor rgb="FF0000FF"/>
   </sheetPr>
-  <dimension ref="A1:N397"/>
+  <dimension ref="A1:S397"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
@@ -973,11 +906,16 @@
     <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" customWidth="1"/>
     <col min="6" max="6" width="4.140625" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" customWidth="1"/>
+    <col min="7" max="7" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" customWidth="1"/>
+    <col min="10" max="10" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.140625" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" customWidth="1"/>
+    <col min="16" max="16" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.95">
+    <row r="1" spans="1:19" ht="30">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -998,12 +936,17 @@
       </c>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
-      <c r="L1" t="str">
-        <f>"Before "&amp;L2&amp;":"</f>
+      <c r="L1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="Q1" t="str">
+        <f>"Before "&amp;Q2&amp;":"</f>
         <v>Before MINIFS:</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:19">
       <c r="A2" s="3">
         <v>42651</v>
       </c>
@@ -1020,14 +963,17 @@
         <v>543.29999999999995</v>
       </c>
       <c r="H2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="6" t="str">
-        <f>H2</f>
+      <c r="Q2" s="6" t="str">
+        <f>M2</f>
         <v>MINIFS</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:19">
       <c r="A3" s="3">
         <v>42979</v>
       </c>
@@ -1043,14 +989,15 @@
       <c r="E3" s="5">
         <v>398</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="8"/>
+      <c r="M3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="8" t="s">
+      <c r="Q3" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:19">
       <c r="A4" s="3">
         <v>42708</v>
       </c>
@@ -1078,17 +1025,29 @@
       <c r="J4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="L4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="N4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="O4" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:14">
+      <c r="Q4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
       <c r="A5" s="3">
         <v>42553</v>
       </c>
@@ -1110,20 +1069,26 @@
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
       <c r="J5" s="9"/>
-      <c r="L5" s="9">
-        <f t="array" ref="L5">MIN(IF($B$2:$B$397=$G5,IF($C$2:$C$397=L$4,$E$2:$E$397)))</f>
+      <c r="L5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="Q5" s="9">
+        <f t="array" ref="Q5">MIN(IF($B$2:$B$397=$L5,IF($C$2:$C$397=Q$4,$E$2:$E$397)))</f>
         <v>273.02999999999997</v>
       </c>
-      <c r="M5" s="9">
-        <f t="array" ref="M5">MIN(IF($B$2:$B$397=$G5,IF($C$2:$C$397=M$4,$E$2:$E$397)))</f>
+      <c r="R5" s="9">
+        <f t="array" ref="R5">MIN(IF($B$2:$B$397=$L5,IF($C$2:$C$397=R$4,$E$2:$E$397)))</f>
         <v>239.5</v>
       </c>
-      <c r="N5" s="9">
-        <f t="array" ref="N5">MIN(IF($B$2:$B$397=$G5,IF($C$2:$C$397=N$4,$E$2:$E$397)))</f>
+      <c r="S5" s="9">
+        <f t="array" ref="S5">MIN(IF($B$2:$B$397=$L5,IF($C$2:$C$397=S$4,$E$2:$E$397)))</f>
         <v>295.77999999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:19">
       <c r="A6" s="3">
         <v>43048</v>
       </c>
@@ -1145,20 +1110,26 @@
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
-      <c r="L6" s="9">
-        <f t="array" ref="L6">MIN(IF($B$2:$B$397=$G6,IF($C$2:$C$397=L$4,$E$2:$E$397)))</f>
+      <c r="L6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="Q6" s="9">
+        <f t="array" ref="Q6">MIN(IF($B$2:$B$397=$L6,IF($C$2:$C$397=Q$4,$E$2:$E$397)))</f>
         <v>355.54</v>
       </c>
-      <c r="M6" s="9">
-        <f t="array" ref="M6">MIN(IF($B$2:$B$397=$G6,IF($C$2:$C$397=M$4,$E$2:$E$397)))</f>
+      <c r="R6" s="9">
+        <f t="array" ref="R6">MIN(IF($B$2:$B$397=$L6,IF($C$2:$C$397=R$4,$E$2:$E$397)))</f>
         <v>274.45</v>
       </c>
-      <c r="N6" s="9">
-        <f t="array" ref="N6">MIN(IF($B$2:$B$397=$G6,IF($C$2:$C$397=N$4,$E$2:$E$397)))</f>
+      <c r="S6" s="9">
+        <f t="array" ref="S6">MIN(IF($B$2:$B$397=$L6,IF($C$2:$C$397=S$4,$E$2:$E$397)))</f>
         <v>274.45</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:19">
       <c r="A7" s="3">
         <v>42831</v>
       </c>
@@ -1180,20 +1151,26 @@
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
-      <c r="L7" s="9">
-        <f t="array" ref="L7">MIN(IF($B$2:$B$397=$G7,IF($C$2:$C$397=L$4,$E$2:$E$397)))</f>
+      <c r="L7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="Q7" s="9">
+        <f t="array" ref="Q7">MIN(IF($B$2:$B$397=$L7,IF($C$2:$C$397=Q$4,$E$2:$E$397)))</f>
         <v>498.07</v>
       </c>
-      <c r="M7" s="9">
-        <f t="array" ref="M7">MIN(IF($B$2:$B$397=$G7,IF($C$2:$C$397=M$4,$E$2:$E$397)))</f>
+      <c r="R7" s="9">
+        <f t="array" ref="R7">MIN(IF($B$2:$B$397=$L7,IF($C$2:$C$397=R$4,$E$2:$E$397)))</f>
         <v>1599.05</v>
       </c>
-      <c r="N7" s="9">
-        <f t="array" ref="N7">MIN(IF($B$2:$B$397=$G7,IF($C$2:$C$397=N$4,$E$2:$E$397)))</f>
+      <c r="S7" s="9">
+        <f t="array" ref="S7">MIN(IF($B$2:$B$397=$L7,IF($C$2:$C$397=S$4,$E$2:$E$397)))</f>
         <v>262.14</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:19">
       <c r="A8" s="3">
         <v>42758</v>
       </c>
@@ -1215,20 +1192,26 @@
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
-      <c r="L8" s="9">
-        <f t="array" ref="L8">MIN(IF($B$2:$B$397=$G8,IF($C$2:$C$397=L$4,$E$2:$E$397)))</f>
+      <c r="L8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="Q8" s="9">
+        <f t="array" ref="Q8">MIN(IF($B$2:$B$397=$L8,IF($C$2:$C$397=Q$4,$E$2:$E$397)))</f>
         <v>416.96</v>
       </c>
-      <c r="M8" s="9">
-        <f t="array" ref="M8">MIN(IF($B$2:$B$397=$G8,IF($C$2:$C$397=M$4,$E$2:$E$397)))</f>
+      <c r="R8" s="9">
+        <f t="array" ref="R8">MIN(IF($B$2:$B$397=$L8,IF($C$2:$C$397=R$4,$E$2:$E$397)))</f>
         <v>265.33999999999997</v>
       </c>
-      <c r="N8" s="9">
-        <f t="array" ref="N8">MIN(IF($B$2:$B$397=$G8,IF($C$2:$C$397=N$4,$E$2:$E$397)))</f>
+      <c r="S8" s="9">
+        <f t="array" ref="S8">MIN(IF($B$2:$B$397=$L8,IF($C$2:$C$397=S$4,$E$2:$E$397)))</f>
         <v>246.38</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:19">
       <c r="A9" s="3">
         <v>42810</v>
       </c>
@@ -1250,20 +1233,26 @@
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
-      <c r="L9" s="9">
-        <f t="array" ref="L9">MIN(IF($B$2:$B$397=$G9,IF($C$2:$C$397=L$4,$E$2:$E$397)))</f>
+      <c r="L9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="Q9" s="9">
+        <f t="array" ref="Q9">MIN(IF($B$2:$B$397=$L9,IF($C$2:$C$397=Q$4,$E$2:$E$397)))</f>
         <v>234.03</v>
       </c>
-      <c r="M9" s="9">
-        <f t="array" ref="M9">MIN(IF($B$2:$B$397=$G9,IF($C$2:$C$397=M$4,$E$2:$E$397)))</f>
+      <c r="R9" s="9">
+        <f t="array" ref="R9">MIN(IF($B$2:$B$397=$L9,IF($C$2:$C$397=R$4,$E$2:$E$397)))</f>
         <v>252.04</v>
       </c>
-      <c r="N9" s="9">
-        <f t="array" ref="N9">MIN(IF($B$2:$B$397=$G9,IF($C$2:$C$397=N$4,$E$2:$E$397)))</f>
+      <c r="S9" s="9">
+        <f t="array" ref="S9">MIN(IF($B$2:$B$397=$L9,IF($C$2:$C$397=S$4,$E$2:$E$397)))</f>
         <v>37.9</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:19">
       <c r="A10" s="3">
         <v>43073</v>
       </c>
@@ -1285,20 +1274,26 @@
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
-      <c r="L10" s="9">
-        <f t="array" ref="L10">MIN(IF($B$2:$B$397=$G10,IF($C$2:$C$397=L$4,$E$2:$E$397)))</f>
+      <c r="L10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="Q10" s="9">
+        <f t="array" ref="Q10">MIN(IF($B$2:$B$397=$L10,IF($C$2:$C$397=Q$4,$E$2:$E$397)))</f>
         <v>332.5</v>
       </c>
-      <c r="M10" s="9">
-        <f t="array" ref="M10">MIN(IF($B$2:$B$397=$G10,IF($C$2:$C$397=M$4,$E$2:$E$397)))</f>
+      <c r="R10" s="9">
+        <f t="array" ref="R10">MIN(IF($B$2:$B$397=$L10,IF($C$2:$C$397=R$4,$E$2:$E$397)))</f>
         <v>150</v>
       </c>
-      <c r="N10" s="9">
-        <f t="array" ref="N10">MIN(IF($B$2:$B$397=$G10,IF($C$2:$C$397=N$4,$E$2:$E$397)))</f>
+      <c r="S10" s="9">
+        <f t="array" ref="S10">MIN(IF($B$2:$B$397=$L10,IF($C$2:$C$397=S$4,$E$2:$E$397)))</f>
         <v>275</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:19">
       <c r="A11" s="3">
         <v>42640</v>
       </c>
@@ -1315,7 +1310,7 @@
         <v>1212.57</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:19">
       <c r="A12" s="3">
         <v>42584</v>
       </c>
@@ -1331,17 +1326,17 @@
       <c r="E12" s="5">
         <v>1482.03</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="L12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="L12" t="str">
-        <f>"Before "&amp;L13&amp;":"</f>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="Q12" t="str">
+        <f>"Before "&amp;Q13&amp;":"</f>
         <v>Before MAXIFS:</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:19">
       <c r="A13" s="3">
         <v>42809</v>
       </c>
@@ -1357,15 +1352,15 @@
       <c r="E13" s="5">
         <v>274.45</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="M13" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="L13" s="6" t="str">
-        <f>H13</f>
+      <c r="Q13" s="6" t="str">
+        <f>M13</f>
         <v>MAXIFS</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:19">
       <c r="A14" s="3">
         <v>42732</v>
       </c>
@@ -1381,14 +1376,14 @@
       <c r="E14" s="5">
         <v>451.25</v>
       </c>
-      <c r="H14" s="8" t="s">
+      <c r="M14" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="L14" s="8" t="s">
+      <c r="Q14" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:19">
       <c r="A15" s="3">
         <v>42644</v>
       </c>
@@ -1404,29 +1399,29 @@
       <c r="E15" s="5">
         <v>684.1</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="L15" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="M15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="N15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J15" s="4" t="s">
+      <c r="O15" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L15" s="4" t="s">
+      <c r="Q15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M15" s="4" t="s">
+      <c r="R15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="N15" s="4" t="s">
+      <c r="S15" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:19">
       <c r="A16" s="3">
         <v>42405</v>
       </c>
@@ -1442,26 +1437,26 @@
       <c r="E16" s="5">
         <v>1163.97</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="L16" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="L16" s="9">
-        <f t="array" ref="L16">MAX(IF($B$2:$B$397=$G16,IF($C$2:$C$397=L$15,$E$2:$E$397)))</f>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="Q16" s="9">
+        <f t="array" ref="Q16">MAX(IF($B$2:$B$397=$L16,IF($C$2:$C$397=Q$15,$E$2:$E$397)))</f>
         <v>1185.53</v>
       </c>
-      <c r="M16" s="9">
-        <f t="array" ref="M16">MAX(IF($B$2:$B$397=$G16,IF($C$2:$C$397=M$15,$E$2:$E$397)))</f>
+      <c r="R16" s="9">
+        <f t="array" ref="R16">MAX(IF($B$2:$B$397=$L16,IF($C$2:$C$397=R$15,$E$2:$E$397)))</f>
         <v>701.26</v>
       </c>
-      <c r="N16" s="9">
-        <f t="array" ref="N16">MAX(IF($B$2:$B$397=$G16,IF($C$2:$C$397=N$15,$E$2:$E$397)))</f>
+      <c r="S16" s="9">
+        <f t="array" ref="S16">MAX(IF($B$2:$B$397=$L16,IF($C$2:$C$397=S$15,$E$2:$E$397)))</f>
         <v>1293.3</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:19">
       <c r="A17" s="3">
         <v>42415</v>
       </c>
@@ -1477,26 +1472,26 @@
       <c r="E17" s="5">
         <v>360.1</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="L17" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="L17" s="9">
-        <f t="array" ref="L17">MAX(IF($B$2:$B$397=$G17,IF($C$2:$C$397=L$15,$E$2:$E$397)))</f>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="Q17" s="9">
+        <f t="array" ref="Q17">MAX(IF($B$2:$B$397=$L17,IF($C$2:$C$397=Q$15,$E$2:$E$397)))</f>
         <v>1212.57</v>
       </c>
-      <c r="M17" s="9">
-        <f t="array" ref="M17">MAX(IF($B$2:$B$397=$G17,IF($C$2:$C$397=M$15,$E$2:$E$397)))</f>
+      <c r="R17" s="9">
+        <f t="array" ref="R17">MAX(IF($B$2:$B$397=$L17,IF($C$2:$C$397=R$15,$E$2:$E$397)))</f>
         <v>1616.76</v>
       </c>
-      <c r="N17" s="9">
-        <f t="array" ref="N17">MAX(IF($B$2:$B$397=$G17,IF($C$2:$C$397=N$15,$E$2:$E$397)))</f>
+      <c r="S17" s="9">
+        <f t="array" ref="S17">MAX(IF($B$2:$B$397=$L17,IF($C$2:$C$397=S$15,$E$2:$E$397)))</f>
         <v>1217.56</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:19">
       <c r="A18" s="3">
         <v>42716</v>
       </c>
@@ -1512,26 +1507,26 @@
       <c r="E18" s="5">
         <v>356.25</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="L18" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="L18" s="9">
-        <f t="array" ref="L18">MAX(IF($B$2:$B$397=$G18,IF($C$2:$C$397=L$15,$E$2:$E$397)))</f>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
+      <c r="Q18" s="9">
+        <f t="array" ref="Q18">MAX(IF($B$2:$B$397=$L18,IF($C$2:$C$397=Q$15,$E$2:$E$397)))</f>
         <v>2123.33</v>
       </c>
-      <c r="M18" s="9">
-        <f t="array" ref="M18">MAX(IF($B$2:$B$397=$G18,IF($C$2:$C$397=M$15,$E$2:$E$397)))</f>
+      <c r="R18" s="9">
+        <f t="array" ref="R18">MAX(IF($B$2:$B$397=$L18,IF($C$2:$C$397=R$15,$E$2:$E$397)))</f>
         <v>2505.1799999999998</v>
       </c>
-      <c r="N18" s="9">
-        <f t="array" ref="N18">MAX(IF($B$2:$B$397=$G18,IF($C$2:$C$397=N$15,$E$2:$E$397)))</f>
+      <c r="S18" s="9">
+        <f t="array" ref="S18">MAX(IF($B$2:$B$397=$L18,IF($C$2:$C$397=S$15,$E$2:$E$397)))</f>
         <v>2132.0700000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:19">
       <c r="A19" s="3">
         <v>42773</v>
       </c>
@@ -1547,26 +1542,26 @@
       <c r="E19" s="5">
         <v>455.05</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="L19" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="L19" s="9">
-        <f t="array" ref="L19">MAX(IF($B$2:$B$397=$G19,IF($C$2:$C$397=L$15,$E$2:$E$397)))</f>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="Q19" s="9">
+        <f t="array" ref="Q19">MAX(IF($B$2:$B$397=$L19,IF($C$2:$C$397=Q$15,$E$2:$E$397)))</f>
         <v>957.6</v>
       </c>
-      <c r="M19" s="9">
-        <f t="array" ref="M19">MAX(IF($B$2:$B$397=$G19,IF($C$2:$C$397=M$15,$E$2:$E$397)))</f>
+      <c r="R19" s="9">
+        <f t="array" ref="R19">MAX(IF($B$2:$B$397=$L19,IF($C$2:$C$397=R$15,$E$2:$E$397)))</f>
         <v>1083.0899999999999</v>
       </c>
-      <c r="N19" s="9">
-        <f t="array" ref="N19">MAX(IF($B$2:$B$397=$G19,IF($C$2:$C$397=N$15,$E$2:$E$397)))</f>
+      <c r="S19" s="9">
+        <f t="array" ref="S19">MAX(IF($B$2:$B$397=$L19,IF($C$2:$C$397=S$15,$E$2:$E$397)))</f>
         <v>961.39</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:19">
       <c r="A20" s="3">
         <v>42908</v>
       </c>
@@ -1582,26 +1577,26 @@
       <c r="E20" s="5">
         <v>273.02999999999997</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="L20" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="L20" s="9">
-        <f t="array" ref="L20">MAX(IF($B$2:$B$397=$G20,IF($C$2:$C$397=L$15,$E$2:$E$397)))</f>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="Q20" s="9">
+        <f t="array" ref="Q20">MAX(IF($B$2:$B$397=$L20,IF($C$2:$C$397=Q$15,$E$2:$E$397)))</f>
         <v>1227.96</v>
       </c>
-      <c r="M20" s="9">
-        <f t="array" ref="M20">MAX(IF($B$2:$B$397=$G20,IF($C$2:$C$397=M$15,$E$2:$E$397)))</f>
+      <c r="R20" s="9">
+        <f t="array" ref="R20">MAX(IF($B$2:$B$397=$L20,IF($C$2:$C$397=R$15,$E$2:$E$397)))</f>
         <v>971</v>
       </c>
-      <c r="N20" s="9">
-        <f t="array" ref="N20">MAX(IF($B$2:$B$397=$G20,IF($C$2:$C$397=N$15,$E$2:$E$397)))</f>
+      <c r="S20" s="9">
+        <f t="array" ref="S20">MAX(IF($B$2:$B$397=$L20,IF($C$2:$C$397=S$15,$E$2:$E$397)))</f>
         <v>1227.96</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:19">
       <c r="A21" s="3">
         <v>42822</v>
       </c>
@@ -1617,26 +1612,26 @@
       <c r="E21" s="5">
         <v>1098</v>
       </c>
-      <c r="G21" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="L21" s="9">
-        <f t="array" ref="L21">MAX(IF($B$2:$B$397=$G21,IF($C$2:$C$397=L$15,$E$2:$E$397)))</f>
+      <c r="L21" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="Q21" s="9">
+        <f t="array" ref="Q21">MAX(IF($B$2:$B$397=$L21,IF($C$2:$C$397=Q$15,$E$2:$E$397)))</f>
         <v>1200</v>
       </c>
-      <c r="M21" s="9">
-        <f t="array" ref="M21">MAX(IF($B$2:$B$397=$G21,IF($C$2:$C$397=M$15,$E$2:$E$397)))</f>
+      <c r="R21" s="9">
+        <f t="array" ref="R21">MAX(IF($B$2:$B$397=$L21,IF($C$2:$C$397=R$15,$E$2:$E$397)))</f>
         <v>855</v>
       </c>
-      <c r="N21" s="9">
-        <f t="array" ref="N21">MAX(IF($B$2:$B$397=$G21,IF($C$2:$C$397=N$15,$E$2:$E$397)))</f>
+      <c r="S21" s="9">
+        <f t="array" ref="S21">MAX(IF($B$2:$B$397=$L21,IF($C$2:$C$397=S$15,$E$2:$E$397)))</f>
         <v>1485</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:19">
       <c r="A22" s="3">
         <v>42962</v>
       </c>
@@ -1653,7 +1648,7 @@
         <v>455.05</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:19">
       <c r="A23" s="3">
         <v>42963</v>
       </c>
@@ -1670,7 +1665,7 @@
         <v>664.09</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:19">
       <c r="A24" s="3">
         <v>42650</v>
       </c>
@@ -1687,7 +1682,7 @@
         <v>1279.24</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:19">
       <c r="A25" s="3">
         <v>42658</v>
       </c>
@@ -1703,11 +1698,11 @@
       <c r="E25" s="5">
         <v>2238.6799999999998</v>
       </c>
-      <c r="G25" s="10" t="s">
+      <c r="L25" s="10" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:19">
       <c r="A26" s="3">
         <v>43005</v>
       </c>
@@ -1723,11 +1718,11 @@
       <c r="E26" s="5">
         <v>2595.19</v>
       </c>
-      <c r="G26" s="10" t="s">
+      <c r="L26" s="10" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:19">
       <c r="A27" s="3">
         <v>42522</v>
       </c>
@@ -1744,7 +1739,7 @@
         <v>179.55</v>
       </c>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:19">
       <c r="A28" s="3">
         <v>42934</v>
       </c>
@@ -1761,7 +1756,7 @@
         <v>1278.44</v>
       </c>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:19">
       <c r="A29" s="3">
         <v>43076</v>
       </c>
@@ -1778,7 +1773,7 @@
         <v>1293.3</v>
       </c>
     </row>
-    <row r="30" spans="1:14">
+    <row r="30" spans="1:19">
       <c r="A30" s="3">
         <v>42678</v>
       </c>
@@ -1795,7 +1790,7 @@
         <v>531.74</v>
       </c>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:19">
       <c r="A31" s="3">
         <v>42694</v>
       </c>
@@ -1812,7 +1807,7 @@
         <v>498.75</v>
       </c>
     </row>
-    <row r="32" spans="1:14">
+    <row r="32" spans="1:19">
       <c r="A32" s="3">
         <v>42857</v>
       </c>
@@ -8036,8 +8031,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G25" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="G26" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="L25" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="L26" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8051,7 +8046,7 @@
   <dimension ref="A1:N397"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -15253,8 +15248,8 @@
   </sheetPr>
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:B10"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -15269,12 +15264,12 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="26.1">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
@@ -15297,88 +15292,109 @@
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="24"/>
+      <c r="B10" s="20"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="B11" s="26"/>
+      <c r="B11" s="22" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="B12" s="12">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="15.95" thickBot="1">
-      <c r="A13" s="13" t="s">
+      <c r="A12" s="11">
+        <v>93</v>
+      </c>
+      <c r="B12" s="12" t="str" cm="1">
+        <f t="array" ref="B12">_xlfn.IFS(A12&gt;90,"A",A12&gt;80,"B", A12&gt;70,"C",A12&gt;65,"D", TRUE,"F")</f>
+        <v>A</v>
+      </c>
+      <c r="C12" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(B12)</f>
+        <v>=IFS(A12&gt;90,"A",A12&gt;80,"B", A12&gt;70,"C",A12&gt;65,"D", TRUE,"F")</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" thickBot="1">
+      <c r="A13" s="11">
+        <v>89</v>
+      </c>
+      <c r="B13" s="12" t="str" cm="1">
+        <f t="array" ref="B13">_xlfn.IFS(A13&gt;90,"A",A13&gt;80,"B", A13&gt;70,"C",A13&gt;65,"D", TRUE,"F")</f>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" thickBot="1">
+      <c r="A14" s="11">
+        <v>75</v>
+      </c>
+      <c r="B14" s="12" t="str" cm="1">
+        <f t="array" ref="B14">_xlfn.IFS(A14&gt;90,"A",A14&gt;80,"B", A14&gt;70,"C",A14&gt;65,"D", TRUE,"F")</f>
+        <v>C</v>
+      </c>
+      <c r="E14" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="14">
-        <v>45000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A14" s="15" t="s">
+    </row>
+    <row r="15" spans="1:5" thickTop="1" thickBot="1">
+      <c r="A15" s="11">
+        <v>69</v>
+      </c>
+      <c r="B15" s="12" t="str" cm="1">
+        <f t="array" ref="B15">_xlfn.IFS(A15&gt;90,"A",A15&gt;80,"B", A15&gt;70,"C",A15&gt;65,"D", TRUE,"F")</f>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" thickBot="1">
+      <c r="A16" s="11">
+        <v>55</v>
+      </c>
+      <c r="B16" s="12" t="str" cm="1">
+        <f t="array" ref="B16">_xlfn.IFS(A16&gt;90,"A",A16&gt;80,"B", A16&gt;70,"C",A16&gt;65,"D", TRUE,"F")</f>
+        <v>F</v>
+      </c>
+      <c r="E16" t="s">
         <v>59</v>
-      </c>
-      <c r="B14" s="16">
-        <f>B12-B13</f>
-        <v>5000</v>
-      </c>
-      <c r="E14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="17.100000000000001" thickTop="1" thickBot="1"/>
-    <row r="16" spans="1:5" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A16" s="15"/>
-      <c r="B16" s="16"/>
-      <c r="E16" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="15.95" thickTop="1"/>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="13" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="17" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="17" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:1">
@@ -15392,9 +15408,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A23" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
@@ -15404,171 +15419,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <sheetPr>
-    <tabColor rgb="FFFF0000"/>
-  </sheetPr>
-  <dimension ref="A1:E24"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="26.1">
-      <c r="A2" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="B10" s="24"/>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="B11" s="26"/>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="B12" s="12">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="15.95" thickBot="1">
-      <c r="A13" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="B13" s="14">
-        <v>45000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A14" s="15" t="str">
-        <f>IF(B12&gt;B13,"Profit",IF(B13&gt;B12,"Loss","Break Even"))</f>
-        <v>Profit</v>
-      </c>
-      <c r="B14" s="16">
-        <f>ABS(B12-B13)</f>
-        <v>5000</v>
-      </c>
-      <c r="E14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="17.100000000000001" thickTop="1" thickBot="1"/>
-    <row r="16" spans="1:5" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A16" s="15" t="str">
-        <f>_xlfn.IFS(B12&gt;B13,"Profit",B13&gt;B12,"Loss",B13=B12,"Break Even")</f>
-        <v>Profit</v>
-      </c>
-      <c r="B16" s="16">
-        <f>ABS(B12-B13)</f>
-        <v>5000</v>
-      </c>
-      <c r="E16" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" ht="15.95" thickTop="1"/>
-    <row r="18" spans="1:1">
-      <c r="A18" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="17" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="17" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" s="10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="A23" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-    <hyperlink ref="A24" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
-    <hyperlink ref="A20" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
-    <hyperlink ref="A19" r:id="rId4" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>